<commit_message>
build a random custom bmw vehicle takes you to the design studo
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4832F212-6FF2-433B-BB8A-340689165B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0EA290-C7FF-4E69-AC31-104984D73FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="6" activeTab="14" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="7" activeTab="15" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
+    <sheet name="nbaCityNameTeamName" sheetId="1" r:id="rId2"/>
     <sheet name="bmwModels" sheetId="3" r:id="rId3"/>
     <sheet name="myTrips" sheetId="4" r:id="rId4"/>
     <sheet name="usaCities" sheetId="5" r:id="rId5"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="203">
   <si>
     <t>City Name</t>
   </si>
@@ -331,9 +331,6 @@
     <t>NBA Teams</t>
   </si>
   <si>
-    <t>Models</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -632,6 +629,36 @@
   </si>
   <si>
     <t>netflix@live.com</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>Z4</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>iX</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>i7</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1059,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,7 +1272,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1282,27 +1309,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1324,142 +1351,142 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1480,22 +1507,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1516,12 +1543,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6879E9-8413-4450-BFB6-832F473E04EB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1545,31 +1572,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B4" s="17">
         <v>213243314</v>
@@ -1577,18 +1604,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1600,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97AC20-6DC1-48C5-9925-A1CA85849984}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1881,36 +1908,112 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DBDB2A-BA3E-4DD2-85D1-84D270436187}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>93</v>
+      <c r="A1" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1929,7 +2032,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1939,72 +2042,72 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2025,17 +2128,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -2045,22 +2148,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2070,7 +2173,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -2100,7 +2203,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2122,37 +2225,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2174,37 +2277,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2227,37 +2330,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2280,37 +2383,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documented bmw test cases
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0EA290-C7FF-4E69-AC31-104984D73FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291AF82C-DEEE-43C1-A3A0-703BFE726770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="7" activeTab="15" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="7" activeTab="14" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="SearchFunction" sheetId="13" r:id="rId13"/>
     <sheet name="AddingToCart" sheetId="14" r:id="rId14"/>
     <sheet name="EmailData" sheetId="15" r:id="rId15"/>
-    <sheet name="Sheet7" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1560,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6879E9-8413-4450-BFB6-832F473E04EB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1619,18 +1618,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C97AC20-6DC1-48C5-9925-A1CA85849984}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
trying to fix espn data provider
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/test/resources/test_data.xlsx
+++ b/com.automationpractice/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.automationpractice\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291AF82C-DEEE-43C1-A3A0-703BFE726770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0066ACA9-0BE5-4CC6-8A4F-364DA79AE88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" firstSheet="7" activeTab="14" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="628" activeTab="1" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
@@ -1559,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6879E9-8413-4450-BFB6-832F473E04EB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -1626,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AF868F-1619-4058-BC1A-5F3E5C88CA24}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>